<commit_message>
Project skeleton classes added
</commit_message>
<xml_diff>
--- a/Work log.xlsx
+++ b/Work log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Időpont</t>
   </si>
@@ -46,13 +46,19 @@
   <si>
     <t>Projekt drótváz + Játék zene szerkesztése</t>
   </si>
+  <si>
+    <t>Össz:</t>
+  </si>
+  <si>
+    <t>Projekt váz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -273,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,10 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -311,7 +317,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -319,6 +325,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D14:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,16 +694,22 @@
         <v>43480</v>
       </c>
       <c r="C8" s="13">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
+      <c r="B9" s="14">
+        <v>43481</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
@@ -782,8 +797,13 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="16">
+        <f>SUM(C3:C25)</f>
+        <v>16</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>